<commit_message>
Updated wheel and made it two seperated
</commit_message>
<xml_diff>
--- a/CAD/parameters.xlsx
+++ b/CAD/parameters.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B558F6-5405-42AD-B6A2-7CAAE834F89D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87340C7-2331-4894-A0A8-F3AE97233C03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23070" yWindow="1035" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>DO_BLDC</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>W_Wall</t>
+  </si>
+  <si>
+    <t>W_WheelCenter</t>
+  </si>
+  <si>
+    <t>T_WheelToShaft</t>
+  </si>
+  <si>
+    <t>Distance between shaft and wheel</t>
   </si>
 </sst>
 </file>
@@ -376,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,6 +485,31 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>